<commit_message>
Added: * defined all necessary components * integrated kwargs, but could have stayed with passing dict_model. solved hashtag error (name spaces) and timeseries format (columns have to be named kW). Better: Add column title to input excel file, or even add feature like in oesmot, so that all profiles provided in one file * simulation runs through
</commit_message>
<xml_diff>
--- a/inputs/test_input_file_v1.xlsx
+++ b/inputs/test_input_file_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="380">
   <si>
     <t xml:space="preserve">User template for the definition of specific…</t>
   </si>
@@ -513,10 +513,7 @@
     <t xml:space="preserve">Distribution efficiency</t>
   </si>
   <si>
-    <t xml:space="preserve">Feed-in tariff (RES)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feed-in tariff (non-RES)</t>
+    <t xml:space="preserve">Feed-in tariff</t>
   </si>
   <si>
     <t xml:space="preserve">Optimize additional capacities</t>
@@ -1839,8 +1836,8 @@
   </sheetPr>
   <dimension ref="B2:H55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2543,7 +2540,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -2606,7 +2603,7 @@
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -2617,7 +2614,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -2661,7 +2658,7 @@
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" s="33" t="n">
         <v>0</v>
@@ -2682,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
@@ -2708,13 +2705,13 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -2722,7 +2719,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -2731,10 +2728,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="35" t="s">
         <v>91</v>
@@ -2744,67 +2741,67 @@
     </row>
     <row r="20" customFormat="false" ht="35.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="48" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="C20" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="21" t="s">
         <v>298</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>299</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="35.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="48" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="C21" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="D21" s="34" t="s">
+      <c r="E21" s="21" t="s">
         <v>301</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>302</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C24" s="53"/>
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="C25" s="53" t="s">
         <v>281</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="61" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C26" s="53" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C27" s="53" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2832,8 +2829,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2857,7 +2854,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -2877,7 +2874,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19"/>
       <c r="B4" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>120</v>
@@ -2934,7 +2931,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19"/>
       <c r="B7" s="42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>120</v>
@@ -2965,10 +2962,10 @@
         <v>4000</v>
       </c>
       <c r="F8" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="G8" s="19" t="s">
         <v>308</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2993,7 +2990,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19"/>
       <c r="B10" s="42" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>120</v>
@@ -3050,7 +3047,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>120</v>
@@ -3107,7 +3104,7 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -3118,7 +3115,7 @@
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
       <c r="B17" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -3149,22 +3146,22 @@
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19"/>
       <c r="B20" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C20" s="45" t="s">
         <v>314</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="D20" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="E20" s="45" t="s">
         <v>316</v>
-      </c>
-      <c r="E20" s="45" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19"/>
       <c r="B21" s="54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C21" s="49" t="n">
         <v>10</v>
@@ -3179,7 +3176,7 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
       <c r="B22" s="54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C22" s="49" t="n">
         <v>10</v>
@@ -3194,7 +3191,7 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19"/>
       <c r="B23" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C23" s="49" t="n">
         <v>10</v>
@@ -3209,7 +3206,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
       <c r="B24" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C24" s="49" t="n">
         <v>10</v>
@@ -3228,13 +3225,13 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19"/>
       <c r="B26" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C27" s="36" t="s">
         <v>90</v>
@@ -3245,7 +3242,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C28" s="49" t="n">
         <v>20</v>
@@ -3256,7 +3253,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C29" s="49" t="n">
         <v>100</v>
@@ -3267,7 +3264,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C30" s="49" t="n">
         <v>95</v>
@@ -3278,18 +3275,18 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C32" s="49" t="n">
         <v>95</v>
@@ -3300,7 +3297,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C33" s="49" t="n">
         <v>1</v>
@@ -3311,43 +3308,43 @@
     </row>
     <row r="34" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="C34" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="31" t="s">
         <v>261</v>
-      </c>
-      <c r="C34" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="48" t="s">
+        <v>323</v>
+      </c>
+      <c r="C35" s="49" t="s">
         <v>324</v>
-      </c>
-      <c r="C35" s="49" t="s">
-        <v>325</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>117</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C36" s="49" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="36" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C37" s="36" t="s">
         <v>90</v>
@@ -3358,7 +3355,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C38" s="49" t="n">
         <v>100</v>
@@ -3369,13 +3366,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C39" s="49" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3422,7 +3419,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -3449,7 +3446,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -3474,7 +3471,7 @@
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19"/>
       <c r="B6" s="42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
@@ -3493,7 +3490,7 @@
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G7" s="19"/>
     </row>
@@ -3508,14 +3505,14 @@
       </c>
       <c r="E8" s="33"/>
       <c r="F8" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
@@ -3534,7 +3531,7 @@
       </c>
       <c r="E10" s="33"/>
       <c r="F10" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G10" s="19"/>
     </row>
@@ -3549,14 +3546,14 @@
       </c>
       <c r="E11" s="33"/>
       <c r="F11" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19"/>
       <c r="B12" s="42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="42"/>
@@ -3575,7 +3572,7 @@
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G13" s="19"/>
     </row>
@@ -3590,14 +3587,14 @@
       </c>
       <c r="E14" s="33"/>
       <c r="F14" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
       <c r="B15" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -3608,7 +3605,7 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -3636,7 +3633,7 @@
     </row>
     <row r="19" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C19" s="45" t="s">
         <v>128</v>
@@ -3648,7 +3645,7 @@
         <v>129</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3659,18 +3656,18 @@
         <v>94</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" s="57" t="s">
         <v>94</v>
       </c>
       <c r="F20" s="63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="49"/>
@@ -3679,7 +3676,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C22" s="49"/>
       <c r="D22" s="49"/>
@@ -3688,7 +3685,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="54" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="49"/>
@@ -3700,14 +3697,14 @@
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="31" t="s">
@@ -3716,7 +3713,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="31" t="s">
@@ -3725,7 +3722,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="31" t="s">
@@ -3734,7 +3731,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="31" t="s">
@@ -3743,16 +3740,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="53" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -3807,7 +3804,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -3834,7 +3831,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -3859,7 +3856,7 @@
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19"/>
       <c r="B6" s="42" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
@@ -3900,7 +3897,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="42" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
@@ -3919,7 +3916,7 @@
       </c>
       <c r="E10" s="33"/>
       <c r="F10" s="34" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G10" s="19"/>
     </row>
@@ -3941,7 +3938,7 @@
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19"/>
       <c r="B12" s="42" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="42"/>
@@ -3982,7 +3979,7 @@
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
       <c r="B15" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -3993,7 +3990,7 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -4019,7 +4016,7 @@
     </row>
     <row r="19" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C19" s="45" t="s">
         <v>128</v>
@@ -4031,7 +4028,7 @@
         <v>129</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4042,18 +4039,18 @@
         <v>94</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E20" s="57" t="s">
         <v>94</v>
       </c>
       <c r="F20" s="63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="54" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="49"/>
@@ -4062,7 +4059,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C22" s="49"/>
       <c r="D22" s="49"/>
@@ -4071,7 +4068,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="54" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="49"/>
@@ -4083,14 +4080,14 @@
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="34" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="31" t="s">
@@ -4099,7 +4096,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="31" t="s">
@@ -4108,7 +4105,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="31" t="s">
@@ -4117,16 +4114,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="31" t="s">
@@ -4135,7 +4132,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="34" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="31" t="s">
@@ -4144,16 +4141,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C32" s="33"/>
       <c r="D32" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="53" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -4208,7 +4205,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -4235,7 +4232,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -4260,7 +4257,7 @@
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19"/>
       <c r="B6" s="42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
@@ -4279,7 +4276,7 @@
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G7" s="19"/>
     </row>
@@ -4294,14 +4291,14 @@
       </c>
       <c r="E8" s="33"/>
       <c r="F8" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
@@ -4320,7 +4317,7 @@
       </c>
       <c r="E10" s="33"/>
       <c r="F10" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G10" s="19"/>
     </row>
@@ -4335,14 +4332,14 @@
       </c>
       <c r="E11" s="33"/>
       <c r="F11" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19"/>
       <c r="B12" s="42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="42"/>
@@ -4361,7 +4358,7 @@
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G13" s="19"/>
     </row>
@@ -4376,14 +4373,14 @@
       </c>
       <c r="E14" s="33"/>
       <c r="F14" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
       <c r="B15" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -4394,7 +4391,7 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -4425,7 +4422,7 @@
     <row r="19" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19"/>
       <c r="B19" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C19" s="45" t="s">
         <v>128</v>
@@ -4437,7 +4434,7 @@
         <v>129</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G19" s="19"/>
     </row>
@@ -4450,19 +4447,19 @@
         <v>94</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" s="57" t="s">
         <v>94</v>
       </c>
       <c r="F20" s="63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="49"/>
@@ -4471,7 +4468,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C22" s="49"/>
       <c r="D22" s="49"/>
@@ -4480,7 +4477,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="54" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="49"/>
@@ -4492,14 +4489,14 @@
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="31" t="s">
@@ -4508,7 +4505,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="31" t="s">
@@ -4517,7 +4514,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="31" t="s">
@@ -4526,7 +4523,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="31" t="s">
@@ -4535,21 +4532,21 @@
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="53" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -4648,7 +4645,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -4707,7 +4704,7 @@
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -4719,7 +4716,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -4769,7 +4766,7 @@
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
@@ -4781,7 +4778,7 @@
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19"/>
       <c r="B14" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="34" t="s">
@@ -4802,7 +4799,7 @@
         <v>135</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -4827,11 +4824,11 @@
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
       <c r="B17" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
@@ -4841,7 +4838,7 @@
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19"/>
       <c r="B18" s="36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C18" s="36"/>
       <c r="D18" s="36"/>
@@ -4853,7 +4850,7 @@
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19"/>
       <c r="B19" s="34" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="34" t="s">
@@ -4866,7 +4863,7 @@
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -4954,7 +4951,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -5009,7 +5006,7 @@
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -5020,7 +5017,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -5066,7 +5063,7 @@
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="34" t="s">
@@ -5107,11 +5104,11 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -5120,7 +5117,7 @@
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
       <c r="B17" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -5131,11 +5128,11 @@
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19"/>
       <c r="B18" s="34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C18" s="33"/>
       <c r="D18" s="34" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
@@ -5188,7 +5185,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="64" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -5215,7 +5212,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -5270,7 +5267,7 @@
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -5281,7 +5278,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -5327,7 +5324,7 @@
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
@@ -5338,7 +5335,7 @@
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19"/>
       <c r="B14" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="34" t="s">
@@ -5379,11 +5376,11 @@
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
       <c r="B17" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
@@ -5403,14 +5400,14 @@
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19"/>
       <c r="B19" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="34" t="s">
         <v>114</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
@@ -5418,14 +5415,14 @@
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19"/>
       <c r="B20" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="34" t="s">
         <v>114</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -5482,7 +5479,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -5502,7 +5499,7 @@
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19"/>
       <c r="B4" s="21" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -5520,7 +5517,7 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="19"/>
@@ -5575,7 +5572,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -5586,7 +5583,7 @@
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19"/>
       <c r="B10" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -5630,7 +5627,7 @@
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19"/>
       <c r="B14" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="34" t="s">
@@ -5671,11 +5668,11 @@
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
       <c r="B17" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
@@ -5683,7 +5680,7 @@
     </row>
     <row r="18" s="65" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -5692,7 +5689,7 @@
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -5704,7 +5701,7 @@
         <v>89</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="35" t="s">
         <v>91</v>
@@ -5714,20 +5711,20 @@
     </row>
     <row r="22" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="48" t="s">
+        <v>367</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>368</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>369</v>
       </c>
       <c r="F22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -5736,7 +5733,7 @@
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -5746,7 +5743,7 @@
         <v>89</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="35" t="s">
         <v>91</v>
@@ -5754,27 +5751,27 @@
     </row>
     <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F28" s="21"/>
     </row>
@@ -5834,7 +5831,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -5861,7 +5858,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -5916,7 +5913,7 @@
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -5927,7 +5924,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -5971,7 +5968,7 @@
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="34" t="s">
@@ -6012,11 +6009,11 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -6024,7 +6021,7 @@
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -6033,7 +6030,7 @@
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -6045,7 +6042,7 @@
         <v>89</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D20" s="35" t="s">
         <v>91</v>
@@ -6055,20 +6052,20 @@
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
@@ -6077,7 +6074,7 @@
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -6087,7 +6084,7 @@
         <v>89</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D25" s="35" t="s">
         <v>91</v>
@@ -6095,27 +6092,27 @@
     </row>
     <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F27" s="21"/>
     </row>
@@ -6373,7 +6370,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -6400,7 +6397,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -6455,7 +6452,7 @@
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -6466,7 +6463,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -6510,7 +6507,7 @@
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="34" t="s">
@@ -6551,11 +6548,11 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -6563,7 +6560,7 @@
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -6572,7 +6569,7 @@
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -6584,7 +6581,7 @@
         <v>89</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D20" s="35" t="s">
         <v>91</v>
@@ -6594,20 +6591,20 @@
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="48" t="s">
+        <v>367</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>368</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>369</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
@@ -6616,7 +6613,7 @@
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -6626,7 +6623,7 @@
         <v>89</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D25" s="35" t="s">
         <v>91</v>
@@ -6634,27 +6631,27 @@
     </row>
     <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F27" s="21"/>
     </row>
@@ -6979,10 +6976,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:K40"/>
+  <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7244,228 +7241,216 @@
       <c r="B25" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="33" t="n">
-        <v>0</v>
+      <c r="C25" s="33" t="s">
+        <v>139</v>
       </c>
       <c r="D25" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="43"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" s="44" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="H28" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="I28" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" s="46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="33" t="n">
+        <v>50</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="43"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="E26" s="43"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" s="44" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="H29" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="I29" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="J29" s="46" t="s">
-        <v>83</v>
+      <c r="I29" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="34" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="33" t="n">
-        <v>50</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>149</v>
-      </c>
       <c r="E30" s="33" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="F30" s="34" t="s">
         <v>87</v>
       </c>
       <c r="G30" s="33" t="n">
-        <v>0.5</v>
+        <v>0.04</v>
       </c>
       <c r="H30" s="34" t="s">
         <v>114</v>
       </c>
       <c r="I30" s="33" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J30" s="34" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="K30" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C31" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="E31" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" s="33" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="I31" s="33" t="n">
-        <v>60</v>
-      </c>
-      <c r="J31" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="K31" s="19" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="18" t="s">
+    <row r="33" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="35" t="s">
         <v>153</v>
       </c>
+      <c r="C33" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="35" t="s">
-        <v>158</v>
+      <c r="B34" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>135</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="48" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D35" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F35" s="34" t="s">
         <v>135</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="48" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D36" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F36" s="34" t="s">
         <v>135</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="C37" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="F37" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="G37" s="19" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="21" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="21" t="s">
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="3" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B37:F37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7500,12 +7485,12 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7517,7 +7502,7 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F5" s="12"/>
     </row>
@@ -7572,17 +7557,17 @@
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7594,7 +7579,7 @@
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F13" s="12"/>
     </row>
@@ -7649,12 +7634,12 @@
     </row>
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7675,7 +7660,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
@@ -7716,23 +7701,23 @@
         <v>117</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="48" t="s">
         <v>182</v>
-      </c>
-      <c r="C26" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
@@ -7775,26 +7760,26 @@
     </row>
     <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" s="49" t="n">
         <v>0</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" s="45" t="s">
         <v>186</v>
-      </c>
-      <c r="C34" s="45" t="s">
-        <v>187</v>
       </c>
       <c r="D34" s="35" t="s">
         <v>91</v>
@@ -7802,67 +7787,67 @@
     </row>
     <row r="35" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="49" t="s">
         <v>188</v>
-      </c>
-      <c r="C35" s="49" t="s">
-        <v>189</v>
       </c>
       <c r="D35" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D36" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F36" s="21"/>
     </row>
     <row r="38" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="42"/>
     </row>
     <row r="40" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C40" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="C40" s="49" t="s">
-        <v>189</v>
-      </c>
       <c r="D40" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C41" s="49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -7913,12 +7898,12 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7930,7 +7915,7 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F5" s="12"/>
     </row>
@@ -7951,7 +7936,7 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" s="49" t="n">
         <v>0</v>
@@ -7963,7 +7948,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7980,22 +7965,22 @@
         <v>0</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8007,7 +7992,7 @@
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F13" s="12"/>
     </row>
@@ -8040,7 +8025,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8057,17 +8042,17 @@
         <v>0</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8088,14 +8073,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C23" s="33" t="n">
         <v>0</v>
@@ -8129,30 +8114,30 @@
         <v>117</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C26" s="33" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C28" s="33" t="n">
         <v>0</v>
@@ -8188,67 +8173,67 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="C33" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" s="34" t="s">
+      <c r="E33" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="E34" s="19" t="s">
         <v>211</v>
-      </c>
-      <c r="C34" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C35" s="33" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C36" s="36"/>
       <c r="D36" s="36"/>
@@ -8260,32 +8245,32 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="34" t="s">
         <v>215</v>
-      </c>
-      <c r="C38" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="E39" s="50" t="s">
         <v>217</v>
-      </c>
-      <c r="C39" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="E39" s="50" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C40" s="33" t="n">
         <v>0</v>
@@ -8294,12 +8279,12 @@
         <v>117</v>
       </c>
       <c r="E40" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
@@ -8307,24 +8292,24 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="34" t="s">
         <v>221</v>
-      </c>
-      <c r="C42" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="34" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C43" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="34" t="s">
         <v>223</v>
-      </c>
-      <c r="C43" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -8377,12 +8362,12 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8394,7 +8379,7 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F5" s="12"/>
     </row>
@@ -8475,7 +8460,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
@@ -8518,13 +8503,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="33" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8536,7 +8521,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C20" s="33" t="n">
         <v>0</v>
@@ -8545,12 +8530,12 @@
         <v>114</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C21" s="33" t="n">
         <v>0</v>
@@ -8559,25 +8544,25 @@
         <v>114</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="52" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>232</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -8585,10 +8570,10 @@
     </row>
     <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>233</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>234</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -8596,10 +8581,10 @@
     </row>
     <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>235</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>236</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -8607,29 +8592,29 @@
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="53" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C31" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="D31" s="45" t="s">
         <v>240</v>
-      </c>
-      <c r="D31" s="45" t="s">
-        <v>241</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>91</v>
       </c>
       <c r="F31" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8641,7 +8626,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C33" s="33" t="n">
         <v>0</v>
@@ -8650,7 +8635,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F33" s="33" t="n">
         <v>0</v>
@@ -8658,7 +8643,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C34" s="33" t="n">
         <v>0</v>
@@ -8667,7 +8652,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F34" s="33" t="n">
         <v>0</v>
@@ -8675,7 +8660,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C35" s="33" t="n">
         <v>0</v>
@@ -8684,7 +8669,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F35" s="33" t="n">
         <v>0</v>
@@ -8695,37 +8680,37 @@
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E37" s="55"/>
     </row>
     <row r="38" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="12"/>
       <c r="C39" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="E39" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C40" s="56" t="n">
         <v>0</v>
@@ -8739,7 +8724,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C41" s="56" t="n">
         <v>0</v>
@@ -8753,7 +8738,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C42" s="56" t="n">
         <v>0</v>
@@ -8767,31 +8752,31 @@
     </row>
     <row r="44" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="12"/>
       <c r="C45" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D45" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="E45" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C46" s="56" t="n">
         <v>0</v>
@@ -8805,7 +8790,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C47" s="56" t="n">
         <v>0</v>
@@ -8819,7 +8804,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C48" s="56" t="n">
         <v>0</v>
@@ -8833,7 +8818,7 @@
     </row>
     <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8844,13 +8829,13 @@
         <v>91</v>
       </c>
       <c r="D51" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="E51" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="E51" s="45" t="s">
+      <c r="F51" s="45" t="s">
         <v>252</v>
-      </c>
-      <c r="F51" s="45" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8862,7 +8847,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="54" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C53" s="57" t="s">
         <v>117</v>
@@ -8879,7 +8864,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C54" s="57" t="s">
         <v>117</v>
@@ -8896,7 +8881,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C55" s="57" t="s">
         <v>117</v>
@@ -8913,10 +8898,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="54" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="57" t="s">
         <v>257</v>
-      </c>
-      <c r="C56" s="57" t="s">
-        <v>258</v>
       </c>
       <c r="D56" s="33" t="n">
         <v>0</v>
@@ -8930,7 +8915,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="54" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C57" s="57" t="s">
         <v>117</v>
@@ -8947,7 +8932,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="54" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C58" s="57" t="s">
         <v>101</v>
@@ -8964,10 +8949,10 @@
     </row>
     <row r="59" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="C59" s="57" t="s">
         <v>261</v>
-      </c>
-      <c r="C59" s="57" t="s">
-        <v>262</v>
       </c>
       <c r="D59" s="33" t="n">
         <v>0</v>
@@ -9021,8 +9006,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9046,7 +9031,7 @@
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="59" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -9066,7 +9051,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19"/>
       <c r="B4" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>120</v>
@@ -9097,10 +9082,10 @@
         <v>7200</v>
       </c>
       <c r="F5" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>265</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9125,7 +9110,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19"/>
       <c r="B7" s="42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>120</v>
@@ -9159,7 +9144,7 @@
         <v>122</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9184,7 +9169,7 @@
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19"/>
       <c r="B10" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -9195,7 +9180,7 @@
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19"/>
       <c r="B11" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -9226,7 +9211,7 @@
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19"/>
       <c r="B14" s="27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>90</v>
@@ -9253,7 +9238,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="34" t="s">
         <v>134</v>
@@ -9262,7 +9247,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -9285,16 +9270,16 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19"/>
       <c r="B18" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="D18" s="34" t="s">
         <v>140</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>141</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
@@ -9312,7 +9297,7 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19"/>
       <c r="B20" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>90</v>
@@ -9339,7 +9324,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
       <c r="B22" s="34" t="s">
         <v>134</v>
@@ -9374,7 +9359,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
       <c r="B24" s="34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C24" s="33" t="n">
         <v>100</v>
@@ -9386,20 +9371,20 @@
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="D25" s="34" t="s">
         <v>140</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -9408,10 +9393,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D28" s="35" t="s">
         <v>91</v>
@@ -9421,59 +9406,59 @@
     </row>
     <row r="29" customFormat="false" ht="23.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="C29" s="33" t="s">
         <v>277</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>278</v>
       </c>
       <c r="D29" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F29" s="21"/>
     </row>
     <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C31" s="53"/>
       <c r="D31" s="53"/>
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" s="53" t="s">
         <v>281</v>
-      </c>
-      <c r="C32" s="53" t="s">
-        <v>282</v>
       </c>
       <c r="D32" s="53"/>
     </row>
     <row r="33" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="C33" s="62" t="s">
         <v>283</v>
-      </c>
-      <c r="C33" s="62" t="s">
-        <v>284</v>
       </c>
       <c r="D33" s="53"/>
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="C34" s="53" t="s">
         <v>285</v>
-      </c>
-      <c r="C34" s="53" t="s">
-        <v>286</v>
       </c>
       <c r="D34" s="53"/>
     </row>
     <row r="35" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="61" t="s">
+        <v>286</v>
+      </c>
+      <c r="C35" s="53" t="s">
         <v>287</v>
-      </c>
-      <c r="C35" s="53" t="s">
-        <v>288</v>
       </c>
       <c r="D35" s="53"/>
     </row>
@@ -9551,7 +9536,7 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="19"/>
@@ -9614,7 +9599,7 @@
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -9625,7 +9610,7 @@
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -9669,7 +9654,7 @@
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
       <c r="B13" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" s="33" t="n">
         <v>0</v>
@@ -9716,13 +9701,13 @@
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
       <c r="B16" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -9730,7 +9715,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -9739,10 +9724,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="35" t="s">
         <v>91</v>
@@ -9752,22 +9737,22 @@
     </row>
     <row r="20" customFormat="false" ht="23.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>135</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="53" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C22" s="53"/>
       <c r="D22" s="53"/>
@@ -9775,30 +9760,30 @@
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="C23" s="53" t="s">
         <v>281</v>
-      </c>
-      <c r="C23" s="53" t="s">
-        <v>282</v>
       </c>
       <c r="D23" s="53"/>
       <c r="E23" s="53"/>
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="61" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D24" s="53"/>
       <c r="E24" s="53"/>
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D25" s="53"/>
       <c r="E25" s="53"/>

</xml_diff>

<commit_message>
Added: * defined all necessary components * integrated kwargs, but could have stayed with passing dict_model. solved hashtag error (name spaces) and timeseries format (columns have to be named kW). Better: Add column title to input excel file, or even add feature like in oesmot, so that all profiles provided in one file * simulation runs through * evaluation complete
left: check results, data output (units!), add fuel source?, graph
</commit_message>
<xml_diff>
--- a/inputs/test_input_file_v1.xlsx
+++ b/inputs/test_input_file_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -594,10 +594,10 @@
     <t xml:space="preserve">Demand 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Reefers (heating and cooling)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demand_reefers.csv</t>
+    <t xml:space="preserve">Habor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand_habor.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Demand 3</t>
@@ -972,7 +972,7 @@
     <t xml:space="preserve">Historical electricity generation</t>
   </si>
   <si>
-    <t xml:space="preserve">pv_gen.csv</t>
+    <t xml:space="preserve">pv_gen_merra2_2014_eff1_tilt40_az180.csv</t>
   </si>
   <si>
     <t xml:space="preserve">electric, timeseries, hourly values, per kWp installed</t>
@@ -1836,7 +1836,7 @@
   </sheetPr>
   <dimension ref="B2:H55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -6683,8 +6683,8 @@
   </sheetPr>
   <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6978,8 +6978,8 @@
   </sheetPr>
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7389,7 +7389,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="48" t="s">
         <v>163</v>
       </c>
@@ -9007,7 +9007,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added: * defined all necessary components * integrated kwargs, but could have stayed with passing dict_model. solved hashtag error (name spaces) and timeseries format (columns have to be named kW). Better: Add column title to input excel file, or even add feature like in oesmot, so that all profiles provided in one file * simulation runs through * evaluation complete * writing to results started (complete for timeseries?) * automatic graphs created
left: check results, data output (units!), add fuel source, calculate kpi
</commit_message>
<xml_diff>
--- a/inputs/test_input_file_v1.xlsx
+++ b/inputs/test_input_file_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -2509,7 +2509,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.54"/>
@@ -3419,7 +3419,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.54"/>
@@ -6705,7 +6705,7 @@
   </sheetPr>
   <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -6924,7 +6924,7 @@
         <v>107</v>
       </c>
       <c r="C25" s="33" t="n">
-        <v>7</v>
+        <v>365</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>108</v>
@@ -7000,7 +7000,7 @@
   </sheetPr>
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>

</xml_diff>